<commit_message>
Elektrisch schema volledig uitgetekend. Footprints toegekend. Twee footprints zelf getekend. Componentenlijst bijgevuld.
</commit_message>
<xml_diff>
--- a/ComponentenlijstRelaisPCB.xlsx
+++ b/ComponentenlijstRelaisPCB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazim\Desktop\POZ\Autonomous_Cart_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE7C1AF-B4F8-4823-8B0D-6EC914F28025}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCE6283-B16C-4285-B1C5-B60E7E15DB9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42B792B0-4795-48E3-A695-BF9CF9749E78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Component</t>
   </si>
@@ -68,7 +68,28 @@
     <t>https://www.conrad.be/p/finder-403170120000-printrelais-12-vdc-12-a-1x-wisselcontact-1-stuks-1560601</t>
   </si>
   <si>
-    <t>Schroef headers</t>
+    <t>Schroef headers 1x3</t>
+  </si>
+  <si>
+    <t>Schroef headers 1x2</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/p/degson-dg308-254-06p-14-00ah-klemschroefblok-082-mm-aantal-polen-6-groen-1-stuks-1327217</t>
+  </si>
+  <si>
+    <t>Schroef headers 1x6</t>
+  </si>
+  <si>
+    <t>Schroef headers 1x8</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/p/degson-dg308-254-08p-14-00ah-klemschroefblok-082-mm-aantal-polen-8-groen-1-stuks-1327226</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/p/degson-dg308-254-02p-14-00ah-klemschroefblok-082-mm-aantal-polen-2-groen-1-stuks-1327242</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/p/degson-dg308-254-03p-14-00ah-klemschroefblok-082-mm-aantal-polen-3-groen-1-stuks-1327224</t>
   </si>
 </sst>
 </file>
@@ -78,7 +99,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ [$€-2]\ * #,##0.00_ ;_ [$€-2]\ * \-#,##0.00_ ;_ [$€-2]\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +127,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -453,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBB21B39-0405-4C12-92C3-2EA1286E89D3}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,7 +492,7 @@
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="94.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="111" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -528,13 +555,81 @@
       <c r="A8" t="s">
         <v>11</v>
       </c>
+      <c r="B8" s="4">
+        <v>0.59</v>
+      </c>
+      <c r="C8">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1.74</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="4">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E6" r:id="rId1" xr:uid="{E44FF811-2EAA-492F-AF2B-1A47297DEC83}"/>
     <hyperlink ref="E7" r:id="rId2" xr:uid="{1C409A2A-6DF9-4701-A10B-6D54B5305CC4}"/>
+    <hyperlink ref="E10" r:id="rId3" xr:uid="{22EC445C-1785-418B-97D7-6DF2EF671717}"/>
+    <hyperlink ref="E11" r:id="rId4" xr:uid="{9EB27A4E-7663-4C68-8039-78300997369D}"/>
+    <hyperlink ref="E9" r:id="rId5" xr:uid="{51E83BEE-E9EE-40BC-B2C0-C2D0F7AC52D0}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{74CA2583-40D6-4293-BABA-75147FF389E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update pcb design update componentenlijst footprints getekent
</commit_message>
<xml_diff>
--- a/ComponentenlijstRelaisPCB.xlsx
+++ b/ComponentenlijstRelaisPCB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazim\Desktop\POZ\Autonomous_Cart_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCE6283-B16C-4285-B1C5-B60E7E15DB9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE1BA6A-B675-463A-899C-747CBBCC0D85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42B792B0-4795-48E3-A695-BF9CF9749E78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Component</t>
   </si>
@@ -74,22 +74,25 @@
     <t>Schroef headers 1x2</t>
   </si>
   <si>
-    <t>https://www.conrad.be/p/degson-dg308-254-06p-14-00ah-klemschroefblok-082-mm-aantal-polen-6-groen-1-stuks-1327217</t>
-  </si>
-  <si>
-    <t>Schroef headers 1x6</t>
-  </si>
-  <si>
-    <t>Schroef headers 1x8</t>
-  </si>
-  <si>
-    <t>https://www.conrad.be/p/degson-dg308-254-08p-14-00ah-klemschroefblok-082-mm-aantal-polen-8-groen-1-stuks-1327226</t>
-  </si>
-  <si>
-    <t>https://www.conrad.be/p/degson-dg308-254-02p-14-00ah-klemschroefblok-082-mm-aantal-polen-2-groen-1-stuks-1327242</t>
-  </si>
-  <si>
-    <t>https://www.conrad.be/p/degson-dg308-254-03p-14-00ah-klemschroefblok-082-mm-aantal-polen-3-groen-1-stuks-1327224</t>
+    <t>Schroef headers 1x4</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/CUI-Devices/TB006-508-14BE?qs=sGAEpiMZZMvZTcaMAxB2AHpdXjUJWjdta3MFIStyIuo0QxXNoLqeaQ%3D%3D</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>Schroef headers 1x14</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/CUI-Devices/TB006-508-02BE?qs=sGAEpiMZZMvZTcaMAxB2AHpdXjUJWjdthU5yE00GqwuGh8iwAbLcpg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/CUI-Devices/TB006-508-04BE?qs=sGAEpiMZZMvZTcaMAxB2AHpdXjUJWjdtxX8qyOuZQe4mznRYcE70wg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/CUI-Devices/TB006-508-03BE?qs=sGAEpiMZZMvZTcaMAxB2AHpdXjUJWjdtVgaMJ9quMmnG8UNjIL2MZA%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -483,7 +486,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,8 +494,8 @@
     <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="111" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="136.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -542,7 +545,7 @@
         <v>5.74</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -556,16 +559,16 @@
         <v>11</v>
       </c>
       <c r="B8" s="4">
-        <v>0.59</v>
+        <v>0.73</v>
       </c>
       <c r="C8">
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -573,13 +576,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="4">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>17</v>
@@ -587,36 +590,36 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="4">
-        <v>1.74</v>
+        <v>0.97</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="4">
-        <v>2.3199999999999998</v>
+        <v>2.48</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -624,10 +627,10 @@
   <hyperlinks>
     <hyperlink ref="E6" r:id="rId1" xr:uid="{E44FF811-2EAA-492F-AF2B-1A47297DEC83}"/>
     <hyperlink ref="E7" r:id="rId2" xr:uid="{1C409A2A-6DF9-4701-A10B-6D54B5305CC4}"/>
-    <hyperlink ref="E10" r:id="rId3" xr:uid="{22EC445C-1785-418B-97D7-6DF2EF671717}"/>
-    <hyperlink ref="E11" r:id="rId4" xr:uid="{9EB27A4E-7663-4C68-8039-78300997369D}"/>
-    <hyperlink ref="E9" r:id="rId5" xr:uid="{51E83BEE-E9EE-40BC-B2C0-C2D0F7AC52D0}"/>
-    <hyperlink ref="E8" r:id="rId6" xr:uid="{74CA2583-40D6-4293-BABA-75147FF389E8}"/>
+    <hyperlink ref="E11" r:id="rId3" xr:uid="{C0E7A543-297E-4B7D-972E-D012F9A13340}"/>
+    <hyperlink ref="E9" r:id="rId4" xr:uid="{90F3F32B-B4EF-482C-911A-E6E15049238D}"/>
+    <hyperlink ref="E10" r:id="rId5" xr:uid="{23EFF7C1-E6C8-43ED-89D2-2BC457DD2F1D}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{786DB20D-08F7-48BD-8DEA-609928934764}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>

</xml_diff>

<commit_message>
update componentenlijst relais PCB
</commit_message>
<xml_diff>
--- a/ComponentenlijstRelaisPCB.xlsx
+++ b/ComponentenlijstRelaisPCB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazim\Desktop\POZ\Autonomous_Cart_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE1BA6A-B675-463A-899C-747CBBCC0D85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5023647D-2FC3-45DF-A4A4-A75CE8E0D732}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42B792B0-4795-48E3-A695-BF9CF9749E78}"/>
   </bookViews>
@@ -486,7 +486,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Componenten lijst update PCB project genaakt voor de actual PCB
</commit_message>
<xml_diff>
--- a/ComponentenlijstRelaisPCB.xlsx
+++ b/ComponentenlijstRelaisPCB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazim\Desktop\POZ\Autonomous_Cart_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5023647D-2FC3-45DF-A4A4-A75CE8E0D732}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F45F4F2-8975-47FB-83C8-607BB1C73DE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42B792B0-4795-48E3-A695-BF9CF9749E78}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="18465" windowHeight="11385" xr2:uid="{42B792B0-4795-48E3-A695-BF9CF9749E78}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Component</t>
   </si>
@@ -59,15 +59,9 @@
     <t>COMPONENTENLIJST RELAIS PCB</t>
   </si>
   <si>
-    <t>https://www.conrad.be/p/finder-405290120000-printrelais-12-vdc-8-a-2x-wisselcontact-1-stuks-502868</t>
-  </si>
-  <si>
     <t>Conrad</t>
   </si>
   <si>
-    <t>https://www.conrad.be/p/finder-403170120000-printrelais-12-vdc-12-a-1x-wisselcontact-1-stuks-1560601</t>
-  </si>
-  <si>
     <t>Schroef headers 1x3</t>
   </si>
   <si>
@@ -93,6 +87,15 @@
   </si>
   <si>
     <t>https://www.mouser.be/ProductDetail/CUI-Devices/TB006-508-03BE?qs=sGAEpiMZZMvZTcaMAxB2AHpdXjUJWjdtVgaMJ9quMmnG8UNjIL2MZA%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/p/finder-403170240000-printrelais-24-vdc-12-a-1x-wisselcontact-1-stuks-1560602</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/p/finder-405290240000-printrelais-24-vdc-8-a-2x-wisselcontact-1-stuks-502882</t>
+  </si>
+  <si>
+    <t>Fly back diode</t>
   </si>
 </sst>
 </file>
@@ -483,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBB21B39-0405-4C12-92C3-2EA1286E89D3}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,10 +534,10 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -548,15 +551,15 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" s="4">
         <v>0.73</v>
@@ -565,15 +568,15 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="4">
         <v>0.5</v>
@@ -582,15 +585,15 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="4">
         <v>0.97</v>
@@ -599,15 +602,15 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" s="4">
         <v>2.48</v>
@@ -616,10 +619,18 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Flyback dioden toegevoeg aan componentenlijst
</commit_message>
<xml_diff>
--- a/ComponentenlijstRelaisPCB.xlsx
+++ b/ComponentenlijstRelaisPCB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazim\Desktop\POZ\Autonomous_Cart_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F45F4F2-8975-47FB-83C8-607BB1C73DE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF664566-49AB-499E-A613-21FE897796B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="735" yWindow="735" windowWidth="18465" windowHeight="11385" xr2:uid="{42B792B0-4795-48E3-A695-BF9CF9749E78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Component</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Fly back diode</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/ROHM-Semiconductor/1SS400CMT2R?qs=sGAEpiMZZMtoHjESLttvkn%252BvjfD1a1Smq9%2FW6eNwDXWDigaLofBvqg%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -489,7 +492,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +501,7 @@
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="136.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="151.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -629,8 +632,17 @@
       <c r="A12" t="s">
         <v>20</v>
       </c>
+      <c r="B12" s="4">
+        <v>1.21</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
       <c r="D12" t="s">
         <v>13</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -642,8 +654,9 @@
     <hyperlink ref="E9" r:id="rId4" xr:uid="{90F3F32B-B4EF-482C-911A-E6E15049238D}"/>
     <hyperlink ref="E10" r:id="rId5" xr:uid="{23EFF7C1-E6C8-43ED-89D2-2BC457DD2F1D}"/>
     <hyperlink ref="E8" r:id="rId6" xr:uid="{786DB20D-08F7-48BD-8DEA-609928934764}"/>
+    <hyperlink ref="E12" r:id="rId7" xr:uid="{F853C941-8D37-48B9-890A-2D93B1BA0419}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update componentenlijst. Alle flyback diodes geintegreerd in de PCB desgin.
</commit_message>
<xml_diff>
--- a/ComponentenlijstRelaisPCB.xlsx
+++ b/ComponentenlijstRelaisPCB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazim\Desktop\POZ\Autonomous_Cart_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF664566-49AB-499E-A613-21FE897796B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA57F3DD-10C3-44F1-B9BC-5D18F368899F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="18465" windowHeight="11385" xr2:uid="{42B792B0-4795-48E3-A695-BF9CF9749E78}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42B792B0-4795-48E3-A695-BF9CF9749E78}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Component</t>
   </si>
@@ -98,7 +98,22 @@
     <t>Fly back diode</t>
   </si>
   <si>
-    <t>https://www.mouser.be/ProductDetail/ROHM-Semiconductor/1SS400CMT2R?qs=sGAEpiMZZMtoHjESLttvkn%252BvjfD1a1Smq9%2FW6eNwDXWDigaLofBvqg%3D%3D</t>
+    <t>https://www.mouser.be/ProductDetail/Diodes-Incorporated/1N4448WQ-7-F?qs=sGAEpiMZZMtoHjESLttvkiVPmB1TVWDoWOW8mzAF96J3zPSzsyGFzg%3D%3D</t>
+  </si>
+  <si>
+    <t>m3 schroef</t>
+  </si>
+  <si>
+    <t>m3 nut</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/tr-fastenings/m3-12-prstmc-z100/screw-pozi-pan-steel-bzp-m3x12/dp/1420391?ost=M3+12+PRSTMC+Z100&amp;ddkey=https%3Anl-BE%2FElement14_Belgium%2Fsearch</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/tr-fastenings/m3-hfa2-s100/full-nut-stainless-steel-a2-m3/dp/1420788?ost=M3+-+HFA2-+S100&amp;ddkey=https%3Anl-BE%2FElement14_Belgium%2Fsearch</t>
+  </si>
+  <si>
+    <t>Farnell</t>
   </si>
 </sst>
 </file>
@@ -489,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBB21B39-0405-4C12-92C3-2EA1286E89D3}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +516,7 @@
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="151.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="172" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -633,7 +648,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="4">
-        <v>1.21</v>
+        <v>0.2</v>
       </c>
       <c r="C12">
         <v>15</v>
@@ -643,6 +658,40 @@
       </c>
       <c r="E12" s="3" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="4">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="4">
+        <v>3.48</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -654,9 +703,11 @@
     <hyperlink ref="E9" r:id="rId4" xr:uid="{90F3F32B-B4EF-482C-911A-E6E15049238D}"/>
     <hyperlink ref="E10" r:id="rId5" xr:uid="{23EFF7C1-E6C8-43ED-89D2-2BC457DD2F1D}"/>
     <hyperlink ref="E8" r:id="rId6" xr:uid="{786DB20D-08F7-48BD-8DEA-609928934764}"/>
-    <hyperlink ref="E12" r:id="rId7" xr:uid="{F853C941-8D37-48B9-890A-2D93B1BA0419}"/>
+    <hyperlink ref="E12" r:id="rId7" xr:uid="{8FF206DC-5DA1-4D2A-A373-C797BD2DC60A}"/>
+    <hyperlink ref="E13" r:id="rId8" xr:uid="{E61F9E43-FFE6-42C0-AD70-F8B522C88E83}"/>
+    <hyperlink ref="E14" r:id="rId9" xr:uid="{4F2DB020-C013-4BD7-9F77-2CAD45BC878C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>